<commit_message>
Indigenous ECE text update May31#4
</commit_message>
<xml_diff>
--- a/dashboard_loader/indigenous_ece_uploader/indigenous_ece.xlsx
+++ b/dashboard_loader/indigenous_ece_uploader/indigenous_ece.xlsx
@@ -92,10 +92,37 @@
     <t xml:space="preserve">In December 2015, COAG renewed the early childhood education target aiming for 95 per cent of all Indigenous four year-olds enrolled in preschool by 2025. </t>
   </si>
   <si>
-    <t xml:space="preserve">The baseline for this target is 2015. In 2016, 91 per cent of Indigenous children were enrolled in early childhood education in the year before full time school.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">In 2016, the information available suggests that all Indigenous children were enrolled in early childhood education in the year before full time school in Victoria, Western Australia and South Australia. Tasmania and the Australian Capital Territory met the required benchmark of 95 per cent.</t>
+    <t xml:space="preserve">The baseline for this target is 2015. In 2016, 91 per cent of Indigenous children were enrolled in early childhood education in the year before full time school, compared to 87 per cent in the baseline year. </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">In 2016, the information available suggests that all Indigenous children were enrolled in early childhood education </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(ECE)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> in the year before full time school in Victoria, Western Australia and South Australia. Tasmania and the Australian Capital Territory met the required benchmark of 95 per cent.</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Notes</t>
@@ -104,10 +131,102 @@
     <t xml:space="preserve">Proportions are over 100 per cent but displayed as 100 per cent for the following: In 2016, Indigenous children in Vic (102 per cent); WA (103 per cent); SA (104 per cent). </t>
   </si>
   <si>
-    <t xml:space="preserve">Improved data quality in the 2016 NECECC collection, resulting from revisions to the ABS data collection methodology, mean that the 2016 data are not fully comparable to the 2015 data. Significant changes include: amended to data linkage approach to enhace the accuracy of child counts in NECECC, and an expanded child identification strategy in the Child Care Management System (one of the source datasets) has increased the count of children enrolled in a preschool program, as all children at long day care centres (of the appropriate age) are now recorded as enrolled in a preschool program.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Preschool enrolment rates reported under the National Partnership on Universal Access to Preschool vary from the NIRA ECE rates. The NIRA and ROGS enrolment rates are based on state-specific Year Before Full-Time School enrolment rates, the NIRA data also prorates Indigenous status not stated.</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Improved data quality in the 2016 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">National Early Childhood Education and Care Collection (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">NECECC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">collection, resulting from revisions to the ABS data collection methodology, mean that the 2016 data are not fully comparable to the 2015 data. Siginificant changes include: amended to data linkage approach to enha</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">ce the accuracy of child counts in NECECC, and an expanded child identification strategy in the Child Care Management System (one of the source datasets) has increased the count of children enrolled in a preschool program, as all children at long day care centres (of the appropraite age) are now recorded as enrolled in a preschool program.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Preschool enrolment rates reported under the National Partnership on Universal Access to Preschool vary from the NIRA ECE rates. The NIRA and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Report on Government Services</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> enrolment rates are based on state-specific Year Before Full-Time School enrolment rates, the NIRA data also prorates Indigenous status not stated.</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Source</t>
@@ -188,9 +307,9 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FF00B050"/>
-      <name val="Calibri"/>
-      <family val="1"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -261,6 +380,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -274,10 +397,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -341,7 +460,7 @@
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF00B050"/>
+      <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
       <rgbColor rgb="FF993300"/>
@@ -361,7 +480,7 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L19" activeCellId="1" sqref="B11 L19"/>
+      <selection pane="topLeft" activeCell="L19" activeCellId="0" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -569,8 +688,8 @@
   </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -580,7 +699,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.33"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>14</v>
       </c>
@@ -596,7 +715,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
         <v>18</v>
       </c>
@@ -604,11 +723,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="5" t="n">
+      <c r="B4" s="6" t="n">
         <v>2016</v>
       </c>
     </row>
@@ -616,20 +735,20 @@
       <c r="A5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="7"/>
+      <c r="D5" s="8"/>
     </row>
     <row r="6" customFormat="false" ht="44.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3"/>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="7"/>
+      <c r="D6" s="8"/>
     </row>
     <row r="7" customFormat="false" ht="52.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="10" t="s">
         <v>24</v>
       </c>
     </row>
@@ -637,18 +756,18 @@
       <c r="A8" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="7"/>
-    </row>
-    <row r="9" customFormat="false" ht="102.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D8" s="8"/>
+    </row>
+    <row r="9" customFormat="false" ht="103.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3"/>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="72.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="52.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3"/>
       <c r="B10" s="10" t="s">
         <v>28</v>
@@ -658,7 +777,7 @@
       <c r="A11" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="7" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Final final round of changes?
</commit_message>
<xml_diff>
--- a/dashboard_loader/indigenous_ece_uploader/indigenous_ece.xlsx
+++ b/dashboard_loader/indigenous_ece_uploader/indigenous_ece.xlsx
@@ -92,7 +92,7 @@
     <t xml:space="preserve">In December 2015, COAG renewed the early childhood education target aiming for 95 per cent of all Indigenous four year-olds enrolled in preschool by 2025. </t>
   </si>
   <si>
-    <t xml:space="preserve">The baseline for this target is 2015. In 2016, 91 per cent of Indigenous children were enrolled in early childhood education in the year before full time school, compared to 87 per cent in the baseline year. </t>
+    <t xml:space="preserve">The baseline for this target is 2015. In 2016, 91 per cent of Indigenous children were enrolled in early childhood education in the year before full time school. </t>
   </si>
   <si>
     <r>
@@ -355,7 +355,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -373,10 +373,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -688,8 +684,8 @@
   </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -727,7 +723,7 @@
       <c r="A4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="6" t="n">
+      <c r="B4" s="5" t="n">
         <v>2016</v>
       </c>
     </row>
@@ -735,20 +731,20 @@
       <c r="A5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="8"/>
-    </row>
-    <row r="6" customFormat="false" ht="44.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D5" s="7"/>
+    </row>
+    <row r="6" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3"/>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="8"/>
+      <c r="D6" s="7"/>
     </row>
     <row r="7" customFormat="false" ht="52.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="9" t="s">
         <v>24</v>
       </c>
     </row>
@@ -756,20 +752,20 @@
       <c r="A8" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="8"/>
+      <c r="D8" s="7"/>
     </row>
     <row r="9" customFormat="false" ht="103.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3"/>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="9" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="52.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3"/>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="9" t="s">
         <v>28</v>
       </c>
     </row>
@@ -777,7 +773,7 @@
       <c r="A11" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="6" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>